<commit_message>
Add model comparison and performance metrics
Implemented ARIMA, Prophet, Diffusion, and GAM models for Apple stock price forecasting. Added code to compute AIC and MSE for each model, generate performance comparison tables, and visualize in-sample fit and out-of-sample forecast accuracy. Commented out unused revenue data loading and improved code structure for clarity.
</commit_message>
<xml_diff>
--- a/revenue_apple_qurter.xlsx
+++ b/revenue_apple_qurter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efaf1e684c19b4e3/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efaf1e684c19b4e3/Desktop/BEFD project/BEFD-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{981725F4-1909-4917-A2C0-8BCF4D05C643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{72328568-6F43-4F92-9692-66B267382C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22276" windowHeight="13276" xr2:uid="{39FBB582-E66B-4D02-B57D-A5536DB07D65}"/>
   </bookViews>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
-    <t>Quarter Ended</t>
-  </si>
-  <si>
-    <t>Revenue (in Bilions)</t>
-  </si>
-  <si>
     <t>Change</t>
   </si>
   <si>
@@ -217,13 +211,19 @@
   </si>
   <si>
     <t>7.94</t>
+  </si>
+  <si>
+    <t>Quarter_Ended</t>
+  </si>
+  <si>
+    <t>Revenue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +354,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -700,9 +708,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -759,6 +768,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1078,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529BF388-8155-431D-AA98-2473F2C2D83C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1089,228 +1102,229 @@
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>44191</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>44282</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>44373</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>44464</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>44555</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>44646</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>44737</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>44828</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>44926</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>45017</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>45108</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>45199</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>45290</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>45381</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>45472</v>
       </c>
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -1318,13 +1332,13 @@
         <v>45563</v>
       </c>
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1332,13 +1346,13 @@
         <v>45654</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -1346,13 +1360,13 @@
         <v>45745</v>
       </c>
       <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -1360,13 +1374,13 @@
         <v>45836</v>
       </c>
       <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -1374,13 +1388,13 @@
         <v>45927</v>
       </c>
       <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>